<commit_message>
Update addLipidReactions.m, addSLIMEreactions.m, and 15 more files...
</commit_message>
<xml_diff>
--- a/data/biomass/biomassCalculations.xlsx
+++ b/data/biomass/biomassCalculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0aad98ece63395da/Documentos_UFV/LABFIS/Lipomyces/GEM-Lipomyces/data/biomass/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mauricio\Biologia\Doutorado\Edurado_Lipomyces-GEM\GEM-Lipomyces\data\biomass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="329" documentId="11_88CDC94357938579773CB938DC694DAAF14BE76E" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CFE2DD3D-A9E9-44CB-8F26-F3486F7764D5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A07DB7-3D43-4B22-8DE1-85F6CF5D70CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19770" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculations" sheetId="1" r:id="rId1"/>
@@ -52,19 +52,10 @@
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -760,9 +751,6 @@
     <t>C18:3 chain</t>
   </si>
   <si>
-    <t>C16:1</t>
-  </si>
-  <si>
     <t>phosphatidylglycerol backbone</t>
   </si>
   <si>
@@ -775,9 +763,6 @@
     <t>m_0103</t>
   </si>
   <si>
-    <t>Incluir no modelo</t>
-  </si>
-  <si>
     <t>Calculated based on annotation</t>
   </si>
   <si>
@@ -794,6 +779,12 @@
   </si>
   <si>
     <t>Sum of mRNA and  ncRNA</t>
+  </si>
+  <si>
+    <t>C16:1 chain</t>
+  </si>
+  <si>
+    <t>s_3741</t>
   </si>
 </sst>
 </file>
@@ -1139,7 +1130,7 @@
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{E0828B3E-AD27-4566-B29D-06DAADAA13DA}"/>
-    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1546,7 +1537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N77"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D37" workbookViewId="0">
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
@@ -1723,10 +1714,10 @@
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="62" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="J10" s="6"/>
     </row>
@@ -1882,7 +1873,7 @@
     </row>
     <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="62" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1919,11 +1910,11 @@
         <v>89.1</v>
       </c>
       <c r="D20" s="10">
-        <f>B20/$B$40</f>
+        <f t="shared" ref="D20:D39" si="1">B20/$B$40</f>
         <v>5.5534266950701475E-2</v>
       </c>
       <c r="E20" s="15">
-        <f t="shared" ref="E20:E39" si="1">C20*D20</f>
+        <f t="shared" ref="E20:E39" si="2">C20*D20</f>
         <v>4.9481031853075015</v>
       </c>
       <c r="F20" s="23">
@@ -1946,15 +1937,15 @@
         <v>174.2</v>
       </c>
       <c r="D21" s="10">
-        <f>B21/$B$40</f>
+        <f t="shared" si="1"/>
         <v>5.4256110319791259E-2</v>
       </c>
       <c r="E21" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.4514144177076371</v>
       </c>
       <c r="F21" s="23">
-        <f t="shared" ref="F20:F39" si="2">D21*$G$24</f>
+        <f t="shared" ref="F21:F39" si="3">D21*$G$24</f>
         <v>0.10174684284260677</v>
       </c>
       <c r="G21" s="3" t="s">
@@ -1972,15 +1963,15 @@
         <v>132.1</v>
       </c>
       <c r="D22" s="10">
-        <f>B22/$B$40</f>
+        <f t="shared" si="1"/>
         <v>5.1629208526086247E-2</v>
       </c>
       <c r="E22" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.8202184462959927</v>
       </c>
       <c r="F22" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.6820596519534674E-2</v>
       </c>
       <c r="G22" s="17">
@@ -1999,15 +1990,15 @@
         <v>133.1</v>
       </c>
       <c r="D23" s="10">
-        <f>B23/$B$40</f>
+        <f t="shared" si="1"/>
         <v>5.3576695700402105E-2</v>
       </c>
       <c r="E23" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.1310581977235197</v>
       </c>
       <c r="F23" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.1004727321093362</v>
       </c>
       <c r="G23" s="3" t="s">
@@ -2025,15 +2016,15 @@
         <v>121.2</v>
       </c>
       <c r="D24" s="10">
-        <f>B24/$B$40</f>
+        <f t="shared" si="1"/>
         <v>2.9313148374573002E-2</v>
       </c>
       <c r="E24" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.5527535829982479</v>
       </c>
       <c r="F24" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.4971141191478765E-2</v>
       </c>
       <c r="G24" s="7">
@@ -2052,15 +2043,15 @@
         <v>146.19999999999999</v>
       </c>
       <c r="D25" s="10">
-        <f>B25/$B$40</f>
+        <f t="shared" si="1"/>
         <v>5.0547691376854526E-2</v>
       </c>
       <c r="E25" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.3900724792961308</v>
       </c>
       <c r="F25" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.4792420250246825E-2</v>
       </c>
       <c r="G25" s="15"/>
@@ -2076,15 +2067,15 @@
         <v>147.1</v>
       </c>
       <c r="D26" s="10">
-        <f>B26/$B$40</f>
+        <f t="shared" si="1"/>
         <v>5.3797284862541442E-2</v>
       </c>
       <c r="E26" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.9135806032798461</v>
       </c>
       <c r="F26" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.10088640442533314</v>
       </c>
       <c r="G26" s="15"/>
@@ -2100,15 +2091,15 @@
         <v>75.099999999999994</v>
       </c>
       <c r="D27" s="10">
-        <f>B27/$B$40</f>
+        <f t="shared" si="1"/>
         <v>5.4461573367955325E-2</v>
       </c>
       <c r="E27" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.0900641599334442</v>
       </c>
       <c r="F27" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.10213214905693534</v>
       </c>
       <c r="G27" s="15"/>
@@ -2124,15 +2115,15 @@
         <v>155.19999999999999</v>
       </c>
       <c r="D28" s="10">
-        <f>B28/$B$40</f>
+        <f t="shared" si="1"/>
         <v>4.2528329950966177E-2</v>
       </c>
       <c r="E28" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.6003968083899505</v>
       </c>
       <c r="F28" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.9753658682403861E-2</v>
       </c>
       <c r="G28" s="15"/>
@@ -2148,15 +2139,15 @@
         <v>131.19999999999999</v>
       </c>
       <c r="D29" s="10">
-        <f>B29/$B$40</f>
+        <f t="shared" si="1"/>
         <v>5.4079638990079788E-2</v>
       </c>
       <c r="E29" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.0952486354984678</v>
       </c>
       <c r="F29" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.10141590498980921</v>
       </c>
       <c r="G29" s="15"/>
@@ -2172,15 +2163,15 @@
         <v>131.19999999999999</v>
       </c>
       <c r="D30" s="10">
-        <f>B30/$B$40</f>
+        <f t="shared" si="1"/>
         <v>5.5689309618947976E-2</v>
       </c>
       <c r="E30" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.306437422005974</v>
       </c>
       <c r="F30" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.104434530975684</v>
       </c>
       <c r="G30" s="15"/>
@@ -2196,15 +2187,15 @@
         <v>146.19999999999999</v>
       </c>
       <c r="D31" s="10">
-        <f>B31/$B$40</f>
+        <f t="shared" si="1"/>
         <v>5.237543014886617E-2</v>
       </c>
       <c r="E31" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.6572878877642339</v>
       </c>
       <c r="F31" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.8219990868507162E-2</v>
       </c>
       <c r="G31" s="15"/>
@@ -2220,15 +2211,15 @@
         <v>149.19999999999999</v>
       </c>
       <c r="D32" s="10">
-        <f>B32/$B$40</f>
+        <f t="shared" si="1"/>
         <v>4.4721616477380155E-2</v>
       </c>
       <c r="E32" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.672465178425119</v>
       </c>
       <c r="F32" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.386674342431627E-2</v>
       </c>
       <c r="G32" s="15"/>
@@ -2244,15 +2235,15 @@
         <v>165.2</v>
       </c>
       <c r="D33" s="10">
-        <f>B33/$B$40</f>
+        <f t="shared" si="1"/>
         <v>5.0812398371421728E-2</v>
       </c>
       <c r="E33" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.3942082109588689</v>
       </c>
       <c r="F33" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.5288827029443149E-2</v>
       </c>
       <c r="G33" s="15"/>
@@ -2268,15 +2259,15 @@
         <v>115.1</v>
       </c>
       <c r="D34" s="10">
-        <f>B34/$B$40</f>
+        <f t="shared" si="1"/>
         <v>5.2463665813721909E-2</v>
       </c>
       <c r="E34" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.0385679351593913</v>
       </c>
       <c r="F34" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.8385459794905941E-2</v>
       </c>
       <c r="G34" s="15"/>
@@ -2292,15 +2283,15 @@
         <v>105.1</v>
       </c>
       <c r="D35" s="10">
-        <f>B35/$B$40</f>
+        <f t="shared" si="1"/>
         <v>5.5457375871327187E-2</v>
       </c>
       <c r="E35" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.8285702040764873</v>
       </c>
       <c r="F35" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.10399958408343579</v>
       </c>
       <c r="G35" s="15"/>
@@ -2316,15 +2307,15 @@
         <v>119.1</v>
       </c>
       <c r="D36" s="10">
-        <f>B36/$B$40</f>
+        <f t="shared" si="1"/>
         <v>5.4302749171215005E-2</v>
       </c>
       <c r="E36" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.4674574262917064</v>
       </c>
       <c r="F36" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.10183430498941755</v>
       </c>
       <c r="G36" s="15"/>
@@ -2340,15 +2331,15 @@
         <v>204.2</v>
       </c>
       <c r="D37" s="10">
-        <f>B37/$B$40</f>
+        <f t="shared" si="1"/>
         <v>3.1430804331110632E-2</v>
       </c>
       <c r="E37" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.4181702444127904</v>
       </c>
       <c r="F37" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.8942395425049358E-2</v>
       </c>
       <c r="G37" s="15"/>
@@ -2364,15 +2355,15 @@
         <v>181.2</v>
       </c>
       <c r="D38" s="10">
-        <f>B38/$B$40</f>
+        <f t="shared" si="1"/>
         <v>4.7913226526161874E-2</v>
       </c>
       <c r="E38" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.6818766465405304</v>
       </c>
       <c r="F38" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.9851990876340534E-2</v>
       </c>
       <c r="G38" s="15"/>
@@ -2388,15 +2379,15 @@
         <v>117.1</v>
       </c>
       <c r="D39" s="10">
-        <f>B39/$B$40</f>
+        <f t="shared" si="1"/>
         <v>5.5109475249896005E-2</v>
       </c>
       <c r="E39" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.4533195517628217</v>
       </c>
       <c r="F39" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.10334716374506349</v>
       </c>
       <c r="G39" s="15"/>
@@ -2426,7 +2417,7 @@
     </row>
     <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="32" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B42" s="32"/>
       <c r="C42" s="32"/>
@@ -2487,11 +2478,11 @@
         <v>190</v>
       </c>
       <c r="B45" s="31">
-        <f t="shared" ref="B45:B48" si="3">G53*(100*$G$44)/$I$53</f>
+        <f t="shared" ref="B45:B48" si="4">G53*(100*$G$44)/$I$53</f>
         <v>12.444444444444445</v>
       </c>
       <c r="C45" s="43">
-        <f t="shared" ref="C45:C48" si="4">B45/100</f>
+        <f t="shared" ref="C45:C48" si="5">B45/100</f>
         <v>0.12444444444444444</v>
       </c>
       <c r="D45" s="10">
@@ -2510,11 +2501,11 @@
         <v>195</v>
       </c>
       <c r="B46" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.0106280193236721</v>
       </c>
       <c r="C46" s="43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.0106280193236719E-2</v>
       </c>
       <c r="D46" s="10">
@@ -2533,11 +2524,11 @@
         <v>193</v>
       </c>
       <c r="B47" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13.120772946859903</v>
       </c>
       <c r="C47" s="43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.13120772946859904</v>
       </c>
       <c r="D47" s="10">
@@ -2556,11 +2547,11 @@
         <v>194</v>
       </c>
       <c r="B48" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.3826086956521744</v>
       </c>
       <c r="C48" s="43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.3826086956521744E-2</v>
       </c>
       <c r="D48" s="10">
@@ -2613,7 +2604,7 @@
         <v>0.25700000000000001</v>
       </c>
       <c r="C52" s="24">
-        <f>B52/100</f>
+        <f t="shared" ref="C52:C61" si="6">B52/100</f>
         <v>2.5700000000000002E-3</v>
       </c>
       <c r="D52" s="40"/>
@@ -2632,7 +2623,7 @@
         <v>16.910599999999999</v>
       </c>
       <c r="C53" s="24">
-        <f>B53/100</f>
+        <f t="shared" si="6"/>
         <v>0.16910599999999998</v>
       </c>
       <c r="D53" s="10"/>
@@ -2654,7 +2645,7 @@
         <v>0.77100000000000002</v>
       </c>
       <c r="C54" s="24">
-        <f>B54/100</f>
+        <f t="shared" si="6"/>
         <v>7.7099999999999998E-3</v>
       </c>
       <c r="D54" s="10"/>
@@ -2675,7 +2666,7 @@
         <v>1.6345970999999999</v>
       </c>
       <c r="C55" s="24">
-        <f>B55/100</f>
+        <f t="shared" si="6"/>
         <v>1.6345971000000001E-2</v>
       </c>
       <c r="D55" s="10"/>
@@ -2696,7 +2687,7 @@
         <v>0.69035340000000001</v>
       </c>
       <c r="C56" s="24">
-        <f>B56/100</f>
+        <f t="shared" si="6"/>
         <v>6.9035340000000002E-3</v>
       </c>
       <c r="D56" s="10"/>
@@ -2715,7 +2706,7 @@
         <v>0.30523889999999998</v>
       </c>
       <c r="C57" s="24">
-        <f>B57/100</f>
+        <f t="shared" si="6"/>
         <v>3.052389E-3</v>
       </c>
       <c r="D57" s="10"/>
@@ -2732,7 +2723,7 @@
         <v>5.7054000000000002E-3</v>
       </c>
       <c r="C58" s="24">
-        <f>B58/100</f>
+        <f t="shared" si="6"/>
         <v>5.7054E-5</v>
       </c>
       <c r="D58" s="10"/>
@@ -2749,7 +2740,7 @@
         <v>4.8495900000000002E-2</v>
       </c>
       <c r="C59" s="24">
-        <f>B59/100</f>
+        <f t="shared" si="6"/>
         <v>4.8495900000000003E-4</v>
       </c>
       <c r="D59" s="10"/>
@@ -2766,7 +2757,7 @@
         <v>2.5700000000000001E-2</v>
       </c>
       <c r="C60" s="24">
-        <f>B60/100</f>
+        <f t="shared" si="6"/>
         <v>2.5700000000000001E-4</v>
       </c>
       <c r="D60" s="10"/>
@@ -2776,14 +2767,14 @@
     </row>
     <row r="61" spans="1:14" s="37" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="27" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B61" s="36">
         <f>7*E64</f>
         <v>1.7989999999999999</v>
       </c>
       <c r="C61" s="24">
-        <f>B61/100</f>
+        <f t="shared" si="6"/>
         <v>1.7989999999999999E-2</v>
       </c>
       <c r="D61" s="35"/>
@@ -2864,7 +2855,7 @@
         <v>9.1749000000000009</v>
       </c>
       <c r="C66" s="31">
-        <f>(100/SUM($B$66:$B$71))*B66</f>
+        <f t="shared" ref="C66:C71" si="7">(100/SUM($B$66:$B$71))*B66</f>
         <v>40.660592255125273</v>
       </c>
       <c r="D66" s="24">
@@ -2886,7 +2877,7 @@
         <v>0.87380000000000002</v>
       </c>
       <c r="C67" s="31">
-        <f>(100/SUM($B$66:$B$71))*B67</f>
+        <f t="shared" si="7"/>
         <v>3.8724373576309783</v>
       </c>
       <c r="D67" s="24">
@@ -2908,11 +2899,11 @@
         <v>0.95090000000000008</v>
       </c>
       <c r="C68" s="31">
-        <f>(100/SUM($B$66:$B$71))*B68</f>
+        <f t="shared" si="7"/>
         <v>4.2141230068337121</v>
       </c>
       <c r="D68" s="24">
-        <f t="shared" ref="D68:D69" si="5">(C68/100)*$E$64</f>
+        <f t="shared" ref="D68:D69" si="8">(C68/100)*$E$64</f>
         <v>1.0830296127562641E-2</v>
       </c>
       <c r="E68" s="32"/>
@@ -2930,11 +2921,11 @@
         <v>11.076700000000001</v>
       </c>
       <c r="C69" s="31">
-        <f>(100/SUM($B$66:$B$71))*B69</f>
+        <f t="shared" si="7"/>
         <v>49.088838268792699</v>
       </c>
       <c r="D69" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.12615831435079725</v>
       </c>
       <c r="E69" s="32"/>
@@ -2952,7 +2943,7 @@
         <v>0.43690000000000001</v>
       </c>
       <c r="C70" s="31">
-        <f>(100/SUM($B$66:$B$71))*B70</f>
+        <f t="shared" si="7"/>
         <v>1.9362186788154891</v>
       </c>
       <c r="D70" s="24">
@@ -2972,7 +2963,7 @@
         <v>5.1400000000000001E-2</v>
       </c>
       <c r="C71" s="31">
-        <f>(100/SUM($B$66:$B$71))*B71</f>
+        <f t="shared" si="7"/>
         <v>0.22779043280182226</v>
       </c>
       <c r="D71" s="24">
@@ -3044,8 +3035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64:XFD64"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection sqref="A1:D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3894,10 +3885,10 @@
     </row>
     <row r="57" spans="1:6" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="52" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B57" s="58" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C57" s="52" t="s">
         <v>92</v>
@@ -3924,10 +3915,10 @@
     </row>
     <row r="59" spans="1:6" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="52" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B59" s="52" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C59" s="52" t="s">
         <v>92</v>
@@ -3998,9 +3989,11 @@
     </row>
     <row r="64" spans="1:6" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="59" t="s">
-        <v>229</v>
-      </c>
-      <c r="B64" s="60"/>
+        <v>239</v>
+      </c>
+      <c r="B64" s="60" t="s">
+        <v>240</v>
+      </c>
       <c r="C64" s="59" t="s">
         <v>91</v>
       </c>
@@ -4008,9 +4001,7 @@
         <f>-Calculations!D67</f>
         <v>-9.9521640091116154E-3</v>
       </c>
-      <c r="F64" s="59" t="s">
-        <v>234</v>
-      </c>
+      <c r="F64" s="59"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
@@ -4062,7 +4053,7 @@
         <v>228</v>
       </c>
       <c r="B68" s="29" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C68" s="53" t="s">
         <v>91</v>

</xml_diff>